<commit_message>
PROS-6350 - SANOFIAE - KPI fix
</commit_message>
<xml_diff>
--- a/Projects/SANOFIAE/Data/Template.xlsx
+++ b/Projects/SANOFIAE/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,9 @@
     <sheet name="Primary&amp;Secondary_POSM" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Primary&amp;Secondary_Facings" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -613,7 +616,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="101">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -840,13 +843,13 @@
     <t xml:space="preserve">Pharmaton</t>
   </si>
   <si>
-    <t xml:space="preserve">VMS</t>
+    <t xml:space="preserve">MVS</t>
   </si>
   <si>
     <t xml:space="preserve">Bronchicum</t>
   </si>
   <si>
-    <t xml:space="preserve">Cough</t>
+    <t xml:space="preserve">Cough &amp; Cold</t>
   </si>
   <si>
     <t xml:space="preserve">Mucosolvan</t>
@@ -861,12 +864,15 @@
     <t xml:space="preserve">Enterogermina</t>
   </si>
   <si>
-    <t xml:space="preserve">DH</t>
+    <t xml:space="preserve">Digestive Health</t>
   </si>
   <si>
     <t xml:space="preserve">Buscopan</t>
   </si>
   <si>
+    <t xml:space="preserve">Pain</t>
+  </si>
+  <si>
     <t xml:space="preserve">SKUs</t>
   </si>
   <si>
@@ -879,19 +885,19 @@
     <t xml:space="preserve">Pharmaton 30 Capsules, Pharmaton 100 Capsules</t>
   </si>
   <si>
-    <t xml:space="preserve">652992,652987</t>
+    <t xml:space="preserve">652992, 652987</t>
   </si>
   <si>
     <t xml:space="preserve">Telfast 30 Tablets X 120mg, Telfast 30 Tablets X 180mg</t>
   </si>
   <si>
-    <t xml:space="preserve">336143,336145</t>
+    <t xml:space="preserve">336143, 336145</t>
   </si>
   <si>
     <t xml:space="preserve">Buscopan  tablets 10mg x 20, Buscopan  tablets 10mg x 50</t>
   </si>
   <si>
-    <t xml:space="preserve">651671,651673</t>
+    <t xml:space="preserve">651671, 651673</t>
   </si>
   <si>
     <t xml:space="preserve">Enterogermina Primary</t>
@@ -900,28 +906,19 @@
     <t xml:space="preserve">PS-006</t>
   </si>
   <si>
-    <t xml:space="preserve">Bronchicum-Mucosolvan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bronchicum-Mucosolvan - Telfast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MVMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRONCHICUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUCOSOLVAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TELFAST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENTEROGERMINA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pain</t>
+    <t xml:space="preserve">Muco/Bronchicum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mucosolvan - Bronchicum - Telfast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cough - Allergy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscopan tablets 10mg x 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscopan tablets 10mg x 50</t>
   </si>
 </sst>
 </file>
@@ -933,7 +930,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -955,13 +952,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="177"/>
     </font>
     <font>
       <b val="true"/>
@@ -1085,13 +1075,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1112,8 +1095,8 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
@@ -1209,7 +1192,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1233,25 +1216,21 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1295,224 +1274,215 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="16" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="22" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="23" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1577,6 +1547,47 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="KPIs"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="MSL"/>
+      <sheetName val="Primary Shelf_Location"/>
+      <sheetName val="Primary_Brand_Blocking"/>
+      <sheetName val="Primary&amp;Secondary_POSM"/>
+      <sheetName val="Primary&amp;Secondary_Facings"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Mucosolvan Syrup 100ml</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Mucosolvan LA 75mg</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>Enterogermina 10 vials of 5ml</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1590,13 +1601,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2057,16 +2068,16 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="42.6315789473684"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="43.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="13" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="11" min="8" style="14" width="10.7125506072875"/>
@@ -2123,7 +2134,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
         <v>23</v>
       </c>
@@ -2158,7 +2169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
         <v>23</v>
       </c>
@@ -2193,7 +2204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
         <v>23</v>
       </c>
@@ -2228,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
         <v>23</v>
       </c>
@@ -2263,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
         <v>23</v>
       </c>
@@ -2298,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
         <v>23</v>
       </c>
@@ -2333,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
         <v>23</v>
       </c>
@@ -2368,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
         <v>23</v>
       </c>
@@ -2403,7 +2414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
         <v>23</v>
       </c>
@@ -2438,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
         <v>23</v>
       </c>
@@ -2452,7 +2463,7 @@
         <v>83</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F12" s="23" t="n">
         <v>1</v>
@@ -2473,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
         <v>23</v>
       </c>
@@ -2487,7 +2498,7 @@
         <v>83</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F13" s="23" t="n">
         <v>1</v>
@@ -2531,25 +2542,25 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="24" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="30.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="24" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="25" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="24" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="31.0647773279352"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="24" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="15" width="8.89068825910931"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="17" t="s">
         <v>63</v>
       </c>
@@ -2566,179 +2577,194 @@
         <v>67</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="G2" s="28" t="s">
+      <c r="F2" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="29"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
+      <c r="G2" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="21"/>
       <c r="E3" s="13"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="33"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="33"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="33"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30" t="s">
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="33"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2762,15 +2788,15 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="36.9554655870445"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="37.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="11" min="6" style="34" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="35" width="8.89068825910931"/>
   </cols>
@@ -2825,7 +2851,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="37" t="s">
         <v>14</v>
       </c>
@@ -2836,10 +2862,10 @@
         <v>75</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F3" s="40" t="n">
         <v>1</v>
@@ -2860,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="37" t="s">
         <v>14</v>
       </c>
@@ -2874,7 +2900,6 @@
         <v>32</v>
       </c>
       <c r="E4" s="39" t="n">
-        <f aca="false">MSL!C5</f>
         <v>653091</v>
       </c>
       <c r="F4" s="40" t="n">
@@ -2896,22 +2921,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="22" t="str">
-        <f aca="false">MSL!E6</f>
-        <v>Cough</v>
+      <c r="C5" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="D5" s="38" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="39" t="n">
-        <f aca="false">MSL!C6</f>
         <v>352016</v>
       </c>
       <c r="F5" s="40" t="n">
@@ -2933,24 +2956,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="22" t="str">
-        <f aca="false">MSL!D7</f>
-        <v>Mucosolvan</v>
-      </c>
-      <c r="C6" s="22" t="str">
-        <f aca="false">MSL!E7</f>
-        <v>Cough</v>
+      <c r="B6" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="D6" s="38" t="str">
-        <f aca="false">MSL!B7</f>
+        <f aca="false">[1]MSL!B7</f>
         <v>Mucosolvan Syrup 100ml</v>
       </c>
       <c r="E6" s="39" t="n">
-        <f aca="false">MSL!C7</f>
         <v>651766</v>
       </c>
       <c r="F6" s="40" t="n">
@@ -2972,24 +2992,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="22" t="str">
-        <f aca="false">MSL!D8</f>
-        <v>Mucosolvan</v>
-      </c>
-      <c r="C7" s="22" t="str">
-        <f aca="false">MSL!E8</f>
-        <v>Cough</v>
+      <c r="B7" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="D7" s="38" t="str">
-        <f aca="false">MSL!B8</f>
+        <f aca="false">[1]MSL!B8</f>
         <v>Mucosolvan LA 75mg</v>
       </c>
       <c r="E7" s="39" t="n">
-        <f aca="false">MSL!C8</f>
         <v>651736</v>
       </c>
       <c r="F7" s="40" t="n">
@@ -3011,23 +3028,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="22" t="str">
-        <f aca="false">MSL!D9</f>
-        <v>Telfast</v>
-      </c>
-      <c r="C8" s="22" t="str">
-        <f aca="false">MSL!E9</f>
-        <v>Allergy</v>
+      <c r="B8" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>80</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F8" s="40" t="n">
         <v>1</v>
@@ -3048,24 +3063,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22" t="str">
-        <f aca="false">MSL!D11</f>
-        <v>Enterogermina</v>
-      </c>
-      <c r="C9" s="22" t="str">
-        <f aca="false">MSL!E11</f>
-        <v>DH</v>
+      <c r="B9" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="D9" s="22" t="str">
-        <f aca="false">MSL!B11</f>
+        <f aca="false">[1]MSL!B11</f>
         <v>Enterogermina 10 vials of 5ml</v>
       </c>
       <c r="E9" s="39" t="n">
-        <f aca="false">MSL!C11</f>
         <v>311922</v>
       </c>
       <c r="F9" s="40" t="n">
@@ -3087,23 +3099,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="34" t="str">
-        <f aca="false">MSL!D12</f>
-        <v>Buscopan</v>
-      </c>
-      <c r="C10" s="34" t="str">
-        <f aca="false">MSL!E12</f>
-        <v>DH</v>
+      <c r="B10" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>84</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="39" t="s">
         <v>92</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>93</v>
       </c>
       <c r="F10" s="40" t="n">
         <v>1</v>
@@ -3146,19 +3156,19 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="42" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="41" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="42" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="42" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="41" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="43" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="41" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="41" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="24" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="42" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3171,25 +3181,25 @@
         <v>63</v>
       </c>
       <c r="G1" s="17"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>67</v>
       </c>
       <c r="F2" s="19" t="s">
@@ -3211,429 +3221,429 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
+      <c r="F3" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="s">
+      <c r="F4" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="s">
+      <c r="F5" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="s">
+      <c r="F6" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="51" t="s">
+      <c r="B7" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="C7" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45" t="s">
+      <c r="F7" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="53" t="s">
+      <c r="F13" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="F11" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="50" t="n">
+      <c r="E14" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="49" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3651,29 +3661,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="55" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="55" width="42.6315789473684"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="55" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="55" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="55" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="55" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="56" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="54" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="54" width="43.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="54" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="54" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="54" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="54" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="55" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="A1" s="56"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
       <c r="F1" s="17" t="s">
         <v>63</v>
       </c>
@@ -3684,19 +3694,19 @@
       <c r="K1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="58" t="s">
+      <c r="A2" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>67</v>
       </c>
       <c r="F2" s="19" t="s">
@@ -3718,756 +3728,740 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="59" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="61" t="n">
+      <c r="C3" s="24" t="n">
         <v>652992</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="63" t="n">
+      <c r="E3" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="63" t="n">
+      <c r="G3" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="63" t="n">
+      <c r="H3" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="K3" s="63" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="59" t="s">
+      <c r="K3" s="60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="61" t="n">
+      <c r="C4" s="24" t="n">
         <v>652987</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="63" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="59" t="s">
+      <c r="E4" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="55" t="n">
+      <c r="C5" s="61" t="n">
         <v>653091</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="F5" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="63" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="59" t="s">
+      <c r="E5" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="55" t="n">
+      <c r="C6" s="61" t="n">
         <v>352016</v>
       </c>
-      <c r="D6" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="55" t="s">
+      <c r="D6" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="63" t="n">
+      <c r="F6" s="60" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="63" t="n">
+      <c r="G6" s="60" t="n">
         <v>3</v>
       </c>
-      <c r="H6" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="63" t="n">
+      <c r="H6" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="60" t="n">
         <v>3</v>
       </c>
-      <c r="K6" s="63" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="59" t="s">
+      <c r="K6" s="60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="55" t="n">
+      <c r="C7" s="61" t="n">
         <v>651766</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="63" t="n">
+      <c r="F7" s="60" t="n">
         <v>3</v>
       </c>
-      <c r="G7" s="63" t="n">
+      <c r="G7" s="60" t="n">
         <v>3</v>
       </c>
-      <c r="H7" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="63" t="n">
+      <c r="H7" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="60" t="n">
         <v>3</v>
       </c>
-      <c r="K7" s="63" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="59" t="s">
+      <c r="K7" s="60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="55" t="n">
+      <c r="C8" s="61" t="n">
         <v>651736</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="61" t="n">
+        <v>336143</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="61" t="n">
+        <v>336145</v>
+      </c>
+      <c r="D10" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="61" t="n">
+        <v>311922</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" s="60" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="C12" s="61" t="n">
+        <v>651671</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="61" t="n">
+        <v>651673</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="61" t="n">
+        <v>652992</v>
+      </c>
+      <c r="D14" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="61" t="n">
+        <v>652987</v>
+      </c>
+      <c r="D15" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="61" t="n">
+        <v>352016</v>
+      </c>
+      <c r="D16" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="63" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="60" t="s">
+      <c r="F16" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="61" t="n">
+        <v>651766</v>
+      </c>
+      <c r="D17" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="61" t="n">
+        <v>651736</v>
+      </c>
+      <c r="D18" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="55" t="n">
+      <c r="C19" s="61" t="n">
         <v>336143</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D19" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="61" t="n">
+        <v>336145</v>
+      </c>
+      <c r="D20" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="61" t="n">
+        <v>311922</v>
+      </c>
+      <c r="D21" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="61" t="n">
+        <v>651671</v>
+      </c>
+      <c r="D22" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="55" t="n">
-        <v>336145</v>
-      </c>
-      <c r="D10" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="55" t="n">
-        <v>311922</v>
-      </c>
-      <c r="D11" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="E11" s="55" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="63" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="63" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="63" t="n">
-        <v>2</v>
-      </c>
-      <c r="I11" s="63" t="n">
-        <v>2</v>
-      </c>
-      <c r="J11" s="63" t="n">
-        <v>2</v>
-      </c>
-      <c r="K11" s="63" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="55" t="n">
-        <v>651671</v>
-      </c>
-      <c r="D12" s="55" t="s">
+      <c r="C23" s="61" t="n">
+        <v>651673</v>
+      </c>
+      <c r="D23" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" s="63" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="55" t="n">
-        <v>651673</v>
-      </c>
-      <c r="D13" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" s="63" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="55" t="n">
-        <v>652992</v>
-      </c>
-      <c r="D14" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="55" t="n">
-        <v>652987</v>
-      </c>
-      <c r="D15" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="55" t="n">
-        <v>352016</v>
-      </c>
-      <c r="D16" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="55" t="n">
-        <v>651766</v>
-      </c>
-      <c r="D17" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="55" t="n">
-        <v>651736</v>
-      </c>
-      <c r="D18" s="55" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="55" t="n">
-        <v>336143</v>
-      </c>
-      <c r="D19" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="55" t="n">
-        <v>336145</v>
-      </c>
-      <c r="D20" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="55" t="n">
-        <v>311922</v>
-      </c>
-      <c r="D21" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="E21" s="0"/>
-      <c r="F21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="55" t="n">
-        <v>651671</v>
-      </c>
-      <c r="D22" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="55" t="n">
-        <v>651673</v>
-      </c>
-      <c r="D23" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="F23" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="63" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="64"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="63"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="64"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="63"/>
+      <c r="E23" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="60" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
SanofiAE - template update
</commit_message>
<xml_diff>
--- a/Projects/SANOFIAE/Data/Template.xlsx
+++ b/Projects/SANOFIAE/Data/Template.xlsx
@@ -24,9 +24,13 @@
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet2!$A$1:$D$59</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet3!$D$2:$E$177</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet3!$D$2:$E$177</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet3!$D$2:$E$177</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet2!$A$1:$D$59</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet2!$A$1:$D$59</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_POSM'!$A$2:$N$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_POSM'!$A$2:$N$2</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$M$32</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$M$32</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1828,7 +1832,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1850,13 +1854,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="177"/>
     </font>
     <font>
       <b val="true"/>
@@ -2179,7 +2176,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2203,25 +2200,21 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="93">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2265,7 +2258,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2273,11 +2266,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2309,7 +2302,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2361,248 +2354,239 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="10" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="10" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="12" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="12" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="10" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="12" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="10" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="12" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="12" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="23" fillId="10" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="12" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="10" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="10" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="12" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="10" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="12" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2696,14 +2680,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4655870445344"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3441295546559"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3036437246964"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0769230769231"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7651821862348"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.080971659919"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.82995951417"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5465587044534"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4453441295547"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4655870445344"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2966,7 +2950,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3169,12 +3153,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.753036437247"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.81376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7732793522267"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.6882591093117"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1174089068826"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2388663967611"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4803,11 +4787,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.81376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0404858299595"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.7570850202429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.4048582995951"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5603,22 +5587,22 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="A3:N38"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="37" width="25.336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="43.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="37" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="18.1174089068826"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="13.4696356275304"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="37" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="11" min="8" style="38" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="39" width="9.54655870445344"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="39" width="11.8744939271255"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="39" width="10.7773279352227"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="39" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="37" width="25.9514170040486"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="44.3198380566802"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="37" width="22.7651821862348"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="18.4898785425101"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="13.834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="37" width="11.2631578947368"/>
+    <col collapsed="false" hidden="false" max="11" min="8" style="38" width="11.2631578947368"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="39" width="9.66801619433198"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="39" width="12.1174089068826"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="39" width="11.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="39" width="9.18218623481781"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6252,7 +6236,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6503,15 +6487,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="25.336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="50" width="21.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="31.3441295546559"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="21.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="50" width="17.3805668016194"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="51" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="25.9514170040486"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="50" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="32.0728744939271"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="50" width="17.753036437247"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="51" width="9.18218623481781"/>
   </cols>
   <sheetData>
-    <row r="1" s="54" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="52"/>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -6567,133 +6551,133 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="55"/>
+      <c r="A3" s="54"/>
       <c r="B3" s="45"/>
       <c r="C3" s="45"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="55"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="59"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="55"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="55"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="59"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="55"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="59"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="55"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="60"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="59"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="55"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="60"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="59"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="55"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="55"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="60"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="59"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="55"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="60"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="59"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="55"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="60"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="55"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="55"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="55"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="59"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="55"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="55"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="60"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6723,19 +6707,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="61" width="21.0607287449393"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="37.582995951417"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="61" width="21.0607287449393"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="61" width="10.7773279352227"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="62" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="60" width="21.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="60" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="60" width="21.4251012145749"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="60" width="11.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="61" width="9.18218623481781"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="A1" s="62"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
       <c r="F1" s="41" t="s">
         <v>372</v>
       </c>
@@ -6793,11 +6777,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="64"/>
+      <c r="A3" s="63"/>
       <c r="B3" s="45"/>
       <c r="C3" s="45"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="66"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="65"/>
       <c r="F3" s="44"/>
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
@@ -6809,11 +6793,11 @@
       <c r="N3" s="44"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="64"/>
+      <c r="A4" s="63"/>
       <c r="B4" s="45"/>
       <c r="C4" s="45"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="66"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44"/>
@@ -6825,11 +6809,11 @@
       <c r="N4" s="44"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="64"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="66"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="65"/>
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
@@ -6841,11 +6825,11 @@
       <c r="N5" s="44"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="64"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="66"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="65"/>
       <c r="F6" s="44"/>
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
@@ -6857,11 +6841,11 @@
       <c r="N6" s="44"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="64"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="65"/>
       <c r="F7" s="44"/>
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
@@ -6873,11 +6857,11 @@
       <c r="N7" s="44"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="64"/>
+      <c r="A8" s="63"/>
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
       <c r="D8" s="45"/>
-      <c r="E8" s="66"/>
+      <c r="E8" s="65"/>
       <c r="F8" s="44"/>
       <c r="G8" s="44"/>
       <c r="H8" s="44"/>
@@ -6889,11 +6873,11 @@
       <c r="N8" s="44"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="64"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
-      <c r="E9" s="66"/>
+      <c r="E9" s="65"/>
       <c r="F9" s="44"/>
       <c r="G9" s="44"/>
       <c r="H9" s="44"/>
@@ -6905,7 +6889,7 @@
       <c r="N9" s="44"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="64"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="0"/>
       <c r="C10" s="0"/>
       <c r="D10" s="0"/>
@@ -6921,11 +6905,11 @@
       <c r="N10" s="44"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="64"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="0"/>
       <c r="C11" s="45"/>
       <c r="D11" s="0"/>
-      <c r="E11" s="67"/>
+      <c r="E11" s="66"/>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
@@ -6937,11 +6921,11 @@
       <c r="N11" s="44"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="64"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="0"/>
       <c r="C12" s="45"/>
       <c r="D12" s="0"/>
-      <c r="E12" s="67"/>
+      <c r="E12" s="66"/>
       <c r="F12" s="44"/>
       <c r="G12" s="44"/>
       <c r="H12" s="44"/>
@@ -6953,11 +6937,11 @@
       <c r="N12" s="44"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="64"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="0"/>
       <c r="C13" s="45"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="67"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="66"/>
       <c r="F13" s="44"/>
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
@@ -6969,11 +6953,11 @@
       <c r="N13" s="44"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="64"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="45"/>
       <c r="C14" s="45"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="68"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="67"/>
       <c r="F14" s="44"/>
       <c r="G14" s="44"/>
       <c r="H14" s="44"/>
@@ -7012,13 +6996,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="69" width="28.7732793522267"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="70" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="71" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="70" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="70" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="69" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="72" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="29.3805668016194"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="68" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="69" width="22.7651821862348"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="68" width="27.2995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="68" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="50" width="11.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="70" width="9.18218623481781"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7040,19 +7024,19 @@
       <c r="N1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="73" t="s">
+      <c r="A2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="71" t="s">
         <v>373</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="71" t="s">
         <v>374</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="71" t="s">
         <v>303</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="71" t="s">
         <v>304</v>
       </c>
       <c r="F2" s="43" t="s">
@@ -7084,574 +7068,574 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="75" t="s">
         <v>247</v>
       </c>
       <c r="E3" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="78" t="n">
+      <c r="F3" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="75" t="s">
         <v>133</v>
       </c>
       <c r="E4" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="78" t="n">
+      <c r="F4" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="75" t="s">
         <v>227</v>
       </c>
       <c r="E5" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="78" t="n">
+      <c r="F5" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="68" t="s">
         <v>390</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="69" t="s">
         <v>391</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="75" t="s">
         <v>227</v>
       </c>
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="78" t="n">
+      <c r="F6" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="77" t="s">
+      <c r="D7" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E7" s="81" t="s">
+      <c r="E7" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" s="78" t="n">
+      <c r="F7" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="73" t="s">
         <v>392</v>
       </c>
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="78" t="s">
         <v>355</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="75" t="s">
         <v>174</v>
       </c>
-      <c r="E8" s="81" t="s">
+      <c r="E8" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="F8" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="78" t="n">
+      <c r="F8" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="82" t="s">
+      <c r="C9" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="77" t="s">
+      <c r="D9" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="81" t="s">
+      <c r="E9" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="78" t="n">
+      <c r="F9" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="75" t="s">
         <v>247</v>
       </c>
       <c r="E10" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" s="78" t="n">
+      <c r="F10" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="73" t="s">
         <v>393</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="77" t="s">
+      <c r="D11" s="75" t="s">
         <v>223</v>
       </c>
       <c r="E11" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" s="78" t="n">
+      <c r="F11" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="73" t="s">
         <v>394</v>
       </c>
-      <c r="C12" s="80" t="s">
+      <c r="C12" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="77" t="s">
+      <c r="D12" s="75" t="s">
         <v>395</v>
       </c>
-      <c r="E12" s="77" t="s">
+      <c r="E12" s="75" t="s">
         <v>396</v>
       </c>
-      <c r="F12" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="78" t="n">
+      <c r="F12" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="83" t="s">
+      <c r="A13" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="80" t="s">
+      <c r="C13" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="77" t="s">
+      <c r="D13" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E13" s="81" t="s">
+      <c r="E13" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="M13" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="78" t="n">
+      <c r="F13" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="83" t="s">
+      <c r="A14" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="76" t="s">
+      <c r="C14" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="77" t="s">
+      <c r="D14" s="75" t="s">
         <v>174</v>
       </c>
-      <c r="E14" s="81" t="s">
+      <c r="E14" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="F14" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="78" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="78" t="n">
+      <c r="F14" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="76" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="83" t="s">
+      <c r="A15" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="82" t="s">
+      <c r="C15" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="77" t="s">
+      <c r="D15" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="E15" s="81" t="s">
+      <c r="E15" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="F15" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="78" t="n">
+      <c r="F15" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7685,21 +7669,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="84" width="31.4655870445344"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="84" width="43.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="84" width="19.0971659919028"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="84" width="17.6234817813765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="84" width="16.6477732793522"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="84" width="10.5263157894737"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="85" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="82" width="32.1983805668016"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="82" width="44.3198380566802"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="82" width="19.587044534413"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="82" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="82" width="17.0161943319838"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="82" width="10.6558704453441"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="83" width="9.18218623481781"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="86"/>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
       <c r="F1" s="41" t="s">
         <v>372</v>
       </c>
@@ -8723,19 +8707,19 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="87" t="s">
+      <c r="A2" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="85" t="s">
         <v>373</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="85" t="s">
         <v>374</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="71" t="s">
         <v>303</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="71" t="s">
         <v>304</v>
       </c>
       <c r="F2" s="43" t="s">
@@ -9776,1202 +9760,1202 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="88" t="s">
+    <row r="3" s="91" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="90" t="n">
+      <c r="C3" s="88" t="n">
         <v>652992</v>
       </c>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="89" t="s">
         <v>247</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="92" t="n">
+      <c r="F3" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="92" t="n">
+      <c r="G3" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="92" t="n">
+      <c r="H3" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="K3" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" s="92" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="88" t="s">
+      <c r="K3" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" s="91" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="90" t="n">
+      <c r="C4" s="88" t="n">
         <v>652987</v>
       </c>
-      <c r="D4" s="91" t="s">
+      <c r="D4" s="89" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="92" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="88" t="s">
+      <c r="F4" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" s="91" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="90" t="n">
+      <c r="C5" s="88" t="n">
         <v>653091</v>
       </c>
-      <c r="D5" s="91" t="s">
+      <c r="D5" s="89" t="s">
         <v>290</v>
       </c>
-      <c r="E5" s="91" t="s">
+      <c r="E5" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="92" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="88" t="s">
+      <c r="F5" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" s="91" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="90" t="n">
+      <c r="C6" s="88" t="n">
         <v>352016</v>
       </c>
-      <c r="D6" s="91" t="s">
+      <c r="D6" s="89" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="92" t="n">
+      <c r="F6" s="90" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="92" t="n">
+      <c r="G6" s="90" t="n">
         <v>3</v>
       </c>
-      <c r="H6" s="92" t="n">
+      <c r="H6" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="92" t="n">
+      <c r="I6" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="J6" s="92" t="n">
+      <c r="J6" s="90" t="n">
         <v>3</v>
       </c>
-      <c r="K6" s="92" t="n">
+      <c r="K6" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="L6" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="92" t="n">
+      <c r="L6" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="90" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="7" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="88" t="s">
+    <row r="7" s="91" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="89" t="s">
+      <c r="B7" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="90" t="n">
+      <c r="C7" s="88" t="n">
         <v>651766</v>
       </c>
-      <c r="D7" s="91" t="s">
+      <c r="D7" s="89" t="s">
         <v>227</v>
       </c>
-      <c r="E7" s="91" t="s">
+      <c r="E7" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="92" t="n">
+      <c r="F7" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="N7" s="92" t="n">
+      <c r="N7" s="90" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="8" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="88" t="s">
+    <row r="8" s="91" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="90" t="n">
+      <c r="C8" s="88" t="n">
         <v>651736</v>
       </c>
-      <c r="D8" s="91" t="s">
+      <c r="D8" s="89" t="s">
         <v>227</v>
       </c>
-      <c r="E8" s="91" t="s">
+      <c r="E8" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="92" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="88" t="s">
+      <c r="F8" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" s="91" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="90" t="n">
+      <c r="C9" s="88" t="n">
         <v>336143</v>
       </c>
-      <c r="D9" s="91" t="s">
+      <c r="D9" s="89" t="s">
         <v>270</v>
       </c>
-      <c r="E9" s="91" t="s">
+      <c r="E9" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" s="92" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="88" t="s">
+      <c r="F9" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" s="91" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="90" t="n">
+      <c r="C10" s="88" t="n">
         <v>336145</v>
       </c>
-      <c r="D10" s="91" t="s">
+      <c r="D10" s="89" t="s">
         <v>270</v>
       </c>
-      <c r="E10" s="91" t="s">
+      <c r="E10" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="N10" s="92" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="88" t="s">
+      <c r="F10" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" s="91" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="90" t="n">
+      <c r="C11" s="88" t="n">
         <v>311922</v>
       </c>
-      <c r="D11" s="91" t="s">
+      <c r="D11" s="89" t="s">
         <v>174</v>
       </c>
-      <c r="E11" s="91" t="s">
+      <c r="E11" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="N11" s="92" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="88" t="s">
+      <c r="F11" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="56" t="s">
         <v>384</v>
       </c>
-      <c r="C12" s="90" t="n">
+      <c r="C12" s="88" t="n">
         <v>599663</v>
       </c>
-      <c r="D12" s="91" t="s">
+      <c r="D12" s="89" t="s">
         <v>174</v>
       </c>
       <c r="E12" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="92" t="n">
+      <c r="F12" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="92" t="n">
+      <c r="G12" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="H12" s="92" t="n">
+      <c r="H12" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="I12" s="92" t="n">
+      <c r="I12" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="J12" s="92" t="n">
+      <c r="J12" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="K12" s="92" t="n">
+      <c r="K12" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="L12" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="92" t="n">
+      <c r="L12" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="90" t="n">
         <v>2</v>
       </c>
-      <c r="N12" s="92" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" s="93" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="88" t="s">
+      <c r="N12" s="90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="56" t="s">
         <v>385</v>
       </c>
-      <c r="C13" s="90" t="n">
+      <c r="C13" s="88" t="n">
         <v>618678</v>
       </c>
-      <c r="D13" s="91" t="s">
+      <c r="D13" s="89" t="s">
         <v>174</v>
       </c>
       <c r="E13" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="92" t="n">
+      <c r="F13" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="90" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="90" t="n">
+      <c r="C14" s="88" t="n">
         <v>651671</v>
       </c>
-      <c r="D14" s="91" t="s">
+      <c r="D14" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="E14" s="91" t="s">
+      <c r="E14" s="89" t="s">
         <v>124</v>
       </c>
-      <c r="F14" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="L14" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="92" t="n">
+      <c r="F14" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="90" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="88" t="s">
+      <c r="A15" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="90" t="n">
+      <c r="C15" s="88" t="n">
         <v>651673</v>
       </c>
-      <c r="D15" s="91" t="s">
+      <c r="D15" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="E15" s="91" t="s">
+      <c r="E15" s="89" t="s">
         <v>124</v>
       </c>
-      <c r="F15" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="92" t="n">
-        <v>1</v>
+      <c r="F15" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="90" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="89" t="s">
+      <c r="B16" s="87" t="s">
         <v>316</v>
       </c>
-      <c r="C16" s="90" t="n">
+      <c r="C16" s="88" t="n">
         <v>565558</v>
       </c>
-      <c r="D16" s="91" t="s">
+      <c r="D16" s="89" t="s">
         <v>211</v>
       </c>
       <c r="E16" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F16" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="N16" s="92" t="n">
+      <c r="F16" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="90" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="89" t="s">
+      <c r="B17" s="87" t="s">
         <v>318</v>
       </c>
-      <c r="C17" s="90" t="n">
+      <c r="C17" s="88" t="n">
         <v>292174</v>
       </c>
-      <c r="D17" s="91" t="s">
+      <c r="D17" s="89" t="s">
         <v>211</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J17" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="L17" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="N17" s="92" t="n">
+      <c r="F17" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="88" t="s">
+      <c r="A18" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="60" t="s">
         <v>386</v>
       </c>
-      <c r="C18" s="90" t="n">
+      <c r="C18" s="88" t="n">
         <v>655324</v>
       </c>
-      <c r="D18" s="91" t="s">
+      <c r="D18" s="89" t="s">
         <v>168</v>
       </c>
       <c r="E18" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="92" t="n">
+      <c r="F18" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="56" t="s">
         <v>387</v>
       </c>
-      <c r="C19" s="90" t="n">
+      <c r="C19" s="88" t="n">
         <v>680065</v>
       </c>
-      <c r="D19" s="91" t="s">
+      <c r="D19" s="89" t="s">
         <v>168</v>
       </c>
       <c r="E19" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F19" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" s="92" t="n">
+      <c r="F19" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="90" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="88" t="s">
+      <c r="A20" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="56" t="s">
         <v>388</v>
       </c>
-      <c r="C20" s="90" t="n">
+      <c r="C20" s="88" t="n">
         <v>674017</v>
       </c>
-      <c r="D20" s="91" t="s">
+      <c r="D20" s="89" t="s">
         <v>168</v>
       </c>
       <c r="E20" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" s="92" t="n">
+      <c r="F20" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="94" t="s">
+      <c r="A21" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="89" t="s">
+      <c r="B21" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="90" t="n">
+      <c r="C21" s="88" t="n">
         <v>652992</v>
       </c>
-      <c r="D21" s="91" t="s">
+      <c r="D21" s="89" t="s">
         <v>247</v>
       </c>
-      <c r="E21" s="91" t="s">
+      <c r="E21" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="F21" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" s="92" t="n">
+      <c r="F21" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="90" t="n">
+      <c r="C22" s="88" t="n">
         <v>652987</v>
       </c>
-      <c r="D22" s="91" t="s">
+      <c r="D22" s="89" t="s">
         <v>247</v>
       </c>
-      <c r="E22" s="91" t="s">
+      <c r="E22" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" s="92" t="n">
+      <c r="F22" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="89" t="s">
+      <c r="B23" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="90" t="n">
+      <c r="C23" s="88" t="n">
         <v>653091</v>
       </c>
-      <c r="D23" s="91" t="s">
+      <c r="D23" s="89" t="s">
         <v>290</v>
       </c>
-      <c r="E23" s="91" t="s">
+      <c r="E23" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="F23" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" s="92" t="n">
+      <c r="F23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="89" t="s">
+      <c r="B24" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="90" t="n">
+      <c r="C24" s="88" t="n">
         <v>352016</v>
       </c>
-      <c r="D24" s="91" t="s">
+      <c r="D24" s="89" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="91" t="s">
+      <c r="E24" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" s="92" t="n">
+      <c r="F24" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="89" t="s">
+      <c r="B25" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="90" t="n">
+      <c r="C25" s="88" t="n">
         <v>651766</v>
       </c>
-      <c r="D25" s="91" t="s">
+      <c r="D25" s="89" t="s">
         <v>227</v>
       </c>
-      <c r="E25" s="91" t="s">
+      <c r="E25" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" s="92" t="n">
+      <c r="F25" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="94" t="s">
+      <c r="A26" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="89" t="s">
+      <c r="B26" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="90" t="n">
+      <c r="C26" s="88" t="n">
         <v>651736</v>
       </c>
-      <c r="D26" s="91" t="s">
+      <c r="D26" s="89" t="s">
         <v>227</v>
       </c>
-      <c r="E26" s="91" t="s">
+      <c r="E26" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" s="92" t="n">
+      <c r="F26" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="94" t="s">
+      <c r="A27" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="90" t="n">
+      <c r="C27" s="88" t="n">
         <v>336143</v>
       </c>
-      <c r="D27" s="91" t="s">
+      <c r="D27" s="89" t="s">
         <v>270</v>
       </c>
-      <c r="E27" s="91" t="s">
+      <c r="E27" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G27" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="M27" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" s="92" t="n">
+      <c r="F27" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="94" t="s">
+      <c r="A28" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="89" t="s">
+      <c r="B28" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="90" t="n">
+      <c r="C28" s="88" t="n">
         <v>336145</v>
       </c>
-      <c r="D28" s="91" t="s">
+      <c r="D28" s="89" t="s">
         <v>270</v>
       </c>
-      <c r="E28" s="91" t="s">
+      <c r="E28" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="M28" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="92" t="n">
+      <c r="F28" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="M28" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="94" t="s">
+      <c r="A29" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="89" t="s">
+      <c r="B29" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="90" t="n">
+      <c r="C29" s="88" t="n">
         <v>311922</v>
       </c>
-      <c r="D29" s="91" t="s">
+      <c r="D29" s="89" t="s">
         <v>174</v>
       </c>
-      <c r="E29" s="91" t="s">
+      <c r="E29" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" s="92" t="n">
+      <c r="F29" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="94" t="s">
+      <c r="A30" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="56" t="s">
         <v>384</v>
       </c>
-      <c r="C30" s="90" t="n">
+      <c r="C30" s="88" t="n">
         <v>599663</v>
       </c>
       <c r="D30" s="45" t="s">
@@ -10980,383 +10964,383 @@
       <c r="E30" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I30" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J30" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="K30" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" s="92" t="n">
+      <c r="F30" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="94" t="s">
+      <c r="A31" s="92" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="49" t="s">
         <v>385</v>
       </c>
-      <c r="C31" s="90" t="n">
+      <c r="C31" s="88" t="n">
         <v>618678</v>
       </c>
-      <c r="D31" s="91" t="s">
+      <c r="D31" s="89" t="s">
         <v>174</v>
       </c>
       <c r="E31" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F31" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J31" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" s="92" t="n">
+      <c r="F31" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="94" t="s">
+      <c r="A32" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="89" t="s">
+      <c r="B32" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="90" t="n">
+      <c r="C32" s="88" t="n">
         <v>651671</v>
       </c>
-      <c r="D32" s="91" t="s">
+      <c r="D32" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="E32" s="91" t="s">
+      <c r="E32" s="89" t="s">
         <v>124</v>
       </c>
-      <c r="F32" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" s="92" t="n">
+      <c r="F32" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="94" t="s">
+      <c r="A33" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="89" t="s">
+      <c r="B33" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="90" t="n">
+      <c r="C33" s="88" t="n">
         <v>651673</v>
       </c>
-      <c r="D33" s="91" t="s">
+      <c r="D33" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="E33" s="91" t="s">
+      <c r="E33" s="89" t="s">
         <v>124</v>
       </c>
-      <c r="F33" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" s="92" t="n">
+      <c r="F33" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="94" t="s">
+      <c r="A34" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="89" t="s">
+      <c r="B34" s="87" t="s">
         <v>316</v>
       </c>
-      <c r="C34" s="90" t="n">
+      <c r="C34" s="88" t="n">
         <v>565558</v>
       </c>
-      <c r="D34" s="91" t="s">
+      <c r="D34" s="89" t="s">
         <v>211</v>
       </c>
-      <c r="E34" s="91" t="s">
+      <c r="E34" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" s="92" t="n">
+      <c r="F34" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="94" t="s">
+      <c r="A35" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="89" t="s">
+      <c r="B35" s="87" t="s">
         <v>318</v>
       </c>
-      <c r="C35" s="90" t="n">
+      <c r="C35" s="88" t="n">
         <v>292174</v>
       </c>
-      <c r="D35" s="91" t="s">
+      <c r="D35" s="89" t="s">
         <v>211</v>
       </c>
-      <c r="E35" s="91" t="s">
+      <c r="E35" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="F35" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L35" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" s="92" t="n">
+      <c r="F35" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="94" t="s">
+      <c r="A36" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="61" t="s">
+      <c r="B36" s="60" t="s">
         <v>386</v>
       </c>
-      <c r="C36" s="90" t="n">
+      <c r="C36" s="88" t="n">
         <v>655324</v>
       </c>
-      <c r="D36" s="91" t="s">
+      <c r="D36" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="E36" s="91" t="s">
+      <c r="E36" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="F36" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K36" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L36" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M36" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" s="92" t="n">
+      <c r="F36" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="57" t="s">
+      <c r="B37" s="56" t="s">
         <v>387</v>
       </c>
-      <c r="C37" s="90" t="n">
+      <c r="C37" s="88" t="n">
         <v>680065</v>
       </c>
-      <c r="D37" s="91" t="s">
+      <c r="D37" s="89" t="s">
         <v>168</v>
       </c>
       <c r="E37" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F37" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J37" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K37" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L37" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" s="92" t="n">
+      <c r="F37" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" s="90" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="94" t="s">
+      <c r="A38" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="56" t="s">
         <v>388</v>
       </c>
-      <c r="C38" s="90" t="n">
+      <c r="C38" s="88" t="n">
         <v>674017</v>
       </c>
-      <c r="D38" s="91" t="s">
+      <c r="D38" s="89" t="s">
         <v>168</v>
       </c>
       <c r="E38" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="F38" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K38" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="M38" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" s="92" t="n">
+      <c r="F38" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" s="90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" s="90" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>